<commit_message>
added regression and cscockpit tests
</commit_message>
<xml_diff>
--- a/src/test/resources/com/rf/test/website/cscockpit/bulk/CSCockpitBulkTest.xlsx
+++ b/src/test/resources/com/rf/test/website/cscockpit/bulk/CSCockpitBulkTest.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10590" windowHeight="5910"/>
   </bookViews>
   <sheets>
     <sheet name="testBulkReturnOrders" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -375,7 +376,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,17 +392,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1000551572</v>
+        <v>1000551790</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1000551574</v>
+        <v>1000551792</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1000551580</v>
+        <v>1000551794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>